<commit_message>
update face collect page
</commit_message>
<xml_diff>
--- a/version.final/students_data/2566.xlsx
+++ b/version.final/students_data/2566.xlsx
@@ -439,8 +439,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>660710073</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>660710073</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -449,13 +451,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Collected</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>660710079</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>660710079</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -469,8 +473,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>660710082</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>660710082</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -484,8 +490,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>660710088</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>660710088</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -499,8 +507,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>660710090</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>660710090</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -514,8 +524,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>660710102</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>660710102</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -529,8 +541,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>660710108</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>660710108</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -544,8 +558,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>660710109</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>660710109</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -559,8 +575,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>660710247</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>660710247</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -574,8 +592,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>660710249</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>660710249</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -589,8 +609,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>660710251</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>660710251</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -604,8 +626,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>660710252</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>660710252</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -619,8 +643,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>660710487</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>660710487</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -634,8 +660,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>660710626</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>660710626</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -649,8 +677,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>660710707</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>660710707</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -664,8 +694,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>660710747</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>660710747</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -679,8 +711,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>660710748</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>660710748</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -694,8 +728,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>660710755</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>660710755</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -709,8 +745,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>660710757</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>660710757</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -724,8 +762,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>660710772</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>660710772</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -739,8 +779,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>660710976</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>660710976</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>

</xml_diff>